<commit_message>
Removed MELTStbl example for docs
</commit_message>
<xml_diff>
--- a/docs/Examples/S6St_Testing/Muth_data_Merged.xlsx
+++ b/docs/Examples/S6St_Testing/Muth_data_Merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\docs\Examples\S6St_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29C688A-FED8-4072-AEB4-5B1D754AEC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0E506B-ADD0-4627-99D2-6D4E3324173E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>Unnamed: 37</t>
   </si>
   <si>
-    <t>H2O</t>
-  </si>
-  <si>
     <t>1s.d.</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>n.a.</t>
+  </si>
+  <si>
+    <t>H2O_Liq</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CN31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="BB12" sqref="BB12"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2080,121 +2080,121 @@
         <v>51</v>
       </c>
       <c r="BB1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="BC1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="CN1" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:92" x14ac:dyDescent="0.35">
@@ -2202,16 +2202,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2">
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2">
         <v>27.025532599999998</v>
@@ -2247,10 +2247,10 @@
         <v>6.2229817769040352E-2</v>
       </c>
       <c r="Q2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S2">
         <v>32</v>
@@ -2262,16 +2262,16 @@
         <v>68</v>
       </c>
       <c r="V2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -2373,16 +2373,16 @@
         <v>0</v>
       </c>
       <c r="BG2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK2">
         <v>38.169542381598838</v>
@@ -2397,10 +2397,10 @@
         <v>3.7176611932427899</v>
       </c>
       <c r="BO2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ2">
         <v>329.01313474908687</v>
@@ -2480,16 +2480,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3">
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3">
         <v>9.36523051</v>
@@ -2525,10 +2525,10 @@
         <v>0.91496216383051898</v>
       </c>
       <c r="Q3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S3">
         <v>33</v>
@@ -2540,16 +2540,16 @@
         <v>73</v>
       </c>
       <c r="V3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W3">
         <v>15</v>
       </c>
       <c r="X3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z3">
         <v>0</v>
@@ -2651,16 +2651,16 @@
         <v>0</v>
       </c>
       <c r="BG3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK3">
         <v>39.744192732047487</v>
@@ -2675,10 +2675,10 @@
         <v>4.5407213903284758</v>
       </c>
       <c r="BO3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ3">
         <v>344.95847330190611</v>
@@ -2758,16 +2758,16 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4">
         <v>14.9879231</v>
@@ -2803,10 +2803,10 @@
         <v>0.39548083233799319</v>
       </c>
       <c r="Q4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S4">
         <v>34</v>
@@ -2818,16 +2818,16 @@
         <v>70</v>
       </c>
       <c r="V4" t="s">
+        <v>132</v>
+      </c>
+      <c r="W4" t="s">
         <v>133</v>
       </c>
-      <c r="W4" t="s">
-        <v>134</v>
-      </c>
       <c r="X4" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y4" t="s">
         <v>132</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>133</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -2929,106 +2929,106 @@
         <v>0</v>
       </c>
       <c r="BG4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BL4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BM4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BN4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BR4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BS4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BT4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BU4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BV4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BW4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BX4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BY4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BZ4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CA4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CB4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CC4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CD4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CE4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CF4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CG4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CH4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CI4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CJ4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CK4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CL4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CM4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CN4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:92" x14ac:dyDescent="0.35">
@@ -3036,16 +3036,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5">
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5">
         <v>2.4291936299999999</v>
@@ -3081,10 +3081,10 @@
         <v>0.39169981916101371</v>
       </c>
       <c r="Q5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S5">
         <v>43</v>
@@ -3096,16 +3096,16 @@
         <v>99</v>
       </c>
       <c r="V5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z5">
         <v>0</v>
@@ -3207,16 +3207,16 @@
         <v>0</v>
       </c>
       <c r="BG5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK5">
         <v>38.023974689346772</v>
@@ -3231,10 +3231,10 @@
         <v>2.1747551134072109</v>
       </c>
       <c r="BO5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ5">
         <v>342.09419632057768</v>
@@ -3314,16 +3314,16 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6">
         <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6">
         <v>4.2422355100000004</v>
@@ -3359,10 +3359,10 @@
         <v>-0.1530333134115871</v>
       </c>
       <c r="Q6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S6">
         <v>44</v>
@@ -3374,16 +3374,16 @@
         <v>50</v>
       </c>
       <c r="V6" t="s">
+        <v>131</v>
+      </c>
+      <c r="W6" t="s">
+        <v>133</v>
+      </c>
+      <c r="X6" t="s">
         <v>132</v>
       </c>
-      <c r="W6" t="s">
-        <v>134</v>
-      </c>
-      <c r="X6" t="s">
-        <v>133</v>
-      </c>
       <c r="Y6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -3485,16 +3485,16 @@
         <v>0</v>
       </c>
       <c r="BG6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK6">
         <v>31.367362881690489</v>
@@ -3509,10 +3509,10 @@
         <v>3.7238699086723068</v>
       </c>
       <c r="BO6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ6">
         <v>267.48228796501462</v>
@@ -3592,16 +3592,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7">
         <v>3.46811231</v>
@@ -3637,10 +3637,10 @@
         <v>0.1873119834353574</v>
       </c>
       <c r="Q7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S7">
         <v>46</v>
@@ -3652,16 +3652,16 @@
         <v>68</v>
       </c>
       <c r="V7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W7">
         <v>17</v>
       </c>
       <c r="X7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -3763,16 +3763,16 @@
         <v>0</v>
       </c>
       <c r="BG7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK7">
         <v>37.000914935558988</v>
@@ -3787,10 +3787,10 @@
         <v>6.2567243500493666</v>
       </c>
       <c r="BO7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ7">
         <v>352.83423278792878</v>
@@ -3870,16 +3870,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8">
         <v>4.25856265</v>
@@ -3915,10 +3915,10 @@
         <v>0.13082012947838351</v>
       </c>
       <c r="Q8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S8">
         <v>47</v>
@@ -3930,16 +3930,16 @@
         <v>199</v>
       </c>
       <c r="V8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W8">
         <v>30</v>
       </c>
       <c r="X8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -4041,16 +4041,16 @@
         <v>0</v>
       </c>
       <c r="BG8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK8">
         <v>35.989276603544077</v>
@@ -4065,10 +4065,10 @@
         <v>2.638480034537606</v>
       </c>
       <c r="BO8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ8">
         <v>262.58828781622577</v>
@@ -4148,16 +4148,16 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9">
         <v>3.0031961900000002</v>
@@ -4193,10 +4193,10 @@
         <v>0.72240736150953921</v>
       </c>
       <c r="Q9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S9">
         <v>49</v>
@@ -4208,16 +4208,16 @@
         <v>124</v>
       </c>
       <c r="V9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W9">
         <v>23</v>
       </c>
       <c r="X9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z9">
         <v>0</v>
@@ -4319,16 +4319,16 @@
         <v>0</v>
       </c>
       <c r="BG9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK9">
         <v>35.521029871422598</v>
@@ -4343,10 +4343,10 @@
         <v>3.890594072974686</v>
       </c>
       <c r="BO9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ9">
         <v>416.17366923363198</v>
@@ -4426,16 +4426,16 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10">
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F10">
         <v>10.5209841</v>
@@ -4471,10 +4471,10 @@
         <v>1.687700667581425</v>
       </c>
       <c r="Q10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S10">
         <v>31</v>
@@ -4486,16 +4486,16 @@
         <v>142</v>
       </c>
       <c r="V10" t="s">
+        <v>132</v>
+      </c>
+      <c r="W10" t="s">
         <v>133</v>
       </c>
-      <c r="W10" t="s">
-        <v>134</v>
-      </c>
       <c r="X10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -4597,16 +4597,16 @@
         <v>0</v>
       </c>
       <c r="BG10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK10">
         <v>29.21396749938555</v>
@@ -4621,10 +4621,10 @@
         <v>3.609883869529853</v>
       </c>
       <c r="BO10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ10">
         <v>547.31158362190047</v>
@@ -4704,16 +4704,16 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11">
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11">
         <v>12.515108100000001</v>
@@ -4749,10 +4749,10 @@
         <v>0.59070339497109092</v>
       </c>
       <c r="Q11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S11">
         <v>35</v>
@@ -4764,16 +4764,16 @@
         <v>105</v>
       </c>
       <c r="V11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W11">
         <v>30</v>
       </c>
       <c r="X11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z11">
         <v>0</v>
@@ -4860,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="BC11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BD11">
         <v>0</v>
@@ -4872,16 +4872,16 @@
         <v>0</v>
       </c>
       <c r="BG11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK11">
         <v>28.20679628271272</v>
@@ -4896,10 +4896,10 @@
         <v>22.59307037763795</v>
       </c>
       <c r="BO11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ11">
         <v>611.21828981207409</v>
@@ -4979,16 +4979,16 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12">
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12">
         <v>14.1435382</v>
@@ -5024,10 +5024,10 @@
         <v>1.181562344963744</v>
       </c>
       <c r="Q12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S12">
         <v>37</v>
@@ -5039,16 +5039,16 @@
         <v>175</v>
       </c>
       <c r="V12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W12">
         <v>43</v>
       </c>
       <c r="X12" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y12" t="s">
         <v>132</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>133</v>
       </c>
       <c r="Z12">
         <v>0</v>
@@ -5150,16 +5150,16 @@
         <v>0</v>
       </c>
       <c r="BG12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK12">
         <v>26.63579698290221</v>
@@ -5174,10 +5174,10 @@
         <v>22.44700736875712</v>
       </c>
       <c r="BO12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ12">
         <v>598.20829930660295</v>
@@ -5257,16 +5257,16 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13">
         <v>15.5100181</v>
@@ -5302,10 +5302,10 @@
         <v>0.93441137034893718</v>
       </c>
       <c r="Q13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S13">
         <v>40</v>
@@ -5317,16 +5317,16 @@
         <v>106</v>
       </c>
       <c r="V13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W13">
         <v>12</v>
       </c>
       <c r="X13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -5428,16 +5428,16 @@
         <v>0</v>
       </c>
       <c r="BG13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK13">
         <v>29.645304229912</v>
@@ -5452,10 +5452,10 @@
         <v>2.7735406262329252</v>
       </c>
       <c r="BO13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ13">
         <v>502.62986375819838</v>
@@ -5535,16 +5535,16 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14">
         <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F14">
         <v>10.2321428</v>
@@ -5580,10 +5580,10 @@
         <v>0.45103082329631938</v>
       </c>
       <c r="Q14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S14">
         <v>42</v>
@@ -5595,16 +5595,16 @@
         <v>157</v>
       </c>
       <c r="V14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W14">
         <v>33</v>
       </c>
       <c r="X14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z14">
         <v>0</v>
@@ -5706,16 +5706,16 @@
         <v>0</v>
       </c>
       <c r="BG14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK14">
         <v>29.850978444450451</v>
@@ -5730,10 +5730,10 @@
         <v>2.52588408913565</v>
       </c>
       <c r="BO14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ14">
         <v>509.02639760211707</v>
@@ -5813,16 +5813,16 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15">
         <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15">
         <v>24.687177399999999</v>
@@ -5858,10 +5858,10 @@
         <v>0.84496962264111541</v>
       </c>
       <c r="Q15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S15">
         <v>43</v>
@@ -5873,16 +5873,16 @@
         <v>182</v>
       </c>
       <c r="V15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W15">
         <v>36</v>
       </c>
       <c r="X15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z15">
         <v>0</v>
@@ -5984,16 +5984,16 @@
         <v>0</v>
       </c>
       <c r="BG15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK15">
         <v>26.47064138546795</v>
@@ -6008,10 +6008,10 @@
         <v>1.9088966431122181</v>
       </c>
       <c r="BO15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ15">
         <v>547.75275620552577</v>
@@ -6091,16 +6091,16 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16">
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F16">
         <v>19.833613400000001</v>
@@ -6136,10 +6136,10 @@
         <v>1.0178894787784061</v>
       </c>
       <c r="Q16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S16">
         <v>44</v>
@@ -6151,16 +6151,16 @@
         <v>124</v>
       </c>
       <c r="V16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W16">
         <v>37</v>
       </c>
       <c r="X16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z16">
         <v>0</v>
@@ -6262,16 +6262,16 @@
         <v>0</v>
       </c>
       <c r="BG16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK16">
         <v>32.1982185018257</v>
@@ -6286,10 +6286,10 @@
         <v>3.5169220839420241</v>
       </c>
       <c r="BO16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ16">
         <v>594.33645723496352</v>
@@ -6369,16 +6369,16 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17">
         <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17">
         <v>15.7119658</v>
@@ -6414,10 +6414,10 @@
         <v>1.201499415607985</v>
       </c>
       <c r="Q17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S17">
         <v>45</v>
@@ -6429,16 +6429,16 @@
         <v>103</v>
       </c>
       <c r="V17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W17">
         <v>26</v>
       </c>
       <c r="X17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -6540,16 +6540,16 @@
         <v>0</v>
       </c>
       <c r="BG17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK17">
         <v>27.957828990121499</v>
@@ -6564,10 +6564,10 @@
         <v>2.4854242886727569</v>
       </c>
       <c r="BO17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ17">
         <v>504.38328682330058</v>
@@ -6647,16 +6647,16 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18">
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18">
         <v>28.259062700000001</v>
@@ -6692,10 +6692,10 @@
         <v>1.981462480172594</v>
       </c>
       <c r="Q18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S18">
         <v>34</v>
@@ -6707,16 +6707,16 @@
         <v>83</v>
       </c>
       <c r="V18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W18">
         <v>25</v>
       </c>
       <c r="X18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z18">
         <v>0</v>
@@ -6818,16 +6818,16 @@
         <v>0</v>
       </c>
       <c r="BG18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK18">
         <v>24.944217453532001</v>
@@ -6842,10 +6842,10 @@
         <v>5.1132634054668129</v>
       </c>
       <c r="BO18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ18">
         <v>1364.1140703829931</v>
@@ -6925,16 +6925,16 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19">
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19">
         <v>17.500456499999999</v>
@@ -6970,10 +6970,10 @@
         <v>1.513325575930268</v>
       </c>
       <c r="Q19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S19">
         <v>24</v>
@@ -6985,16 +6985,16 @@
         <v>133</v>
       </c>
       <c r="V19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W19">
         <v>41</v>
       </c>
       <c r="X19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -7096,16 +7096,16 @@
         <v>0</v>
       </c>
       <c r="BG19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK19">
         <v>26.880975495325028</v>
@@ -7120,10 +7120,10 @@
         <v>2.0821057028422851</v>
       </c>
       <c r="BO19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ19">
         <v>1158.8975882102111</v>
@@ -7203,16 +7203,16 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20">
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F20">
         <v>16.568765800000001</v>
@@ -7248,10 +7248,10 @@
         <v>1.5280233808882939</v>
       </c>
       <c r="Q20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S20">
         <v>25</v>
@@ -7263,16 +7263,16 @@
         <v>144</v>
       </c>
       <c r="V20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W20">
         <v>38</v>
       </c>
       <c r="X20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z20">
         <v>0</v>
@@ -7374,16 +7374,16 @@
         <v>0</v>
       </c>
       <c r="BG20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK20">
         <v>22.87165538428523</v>
@@ -7398,10 +7398,10 @@
         <v>2.3652605950055769</v>
       </c>
       <c r="BO20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ20">
         <v>1431.3457870844061</v>
@@ -7481,16 +7481,16 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21">
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F21">
         <v>13.236040900000001</v>
@@ -7526,10 +7526,10 @@
         <v>1.315035136481066</v>
       </c>
       <c r="Q21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S21">
         <v>26</v>
@@ -7541,16 +7541,16 @@
         <v>109</v>
       </c>
       <c r="V21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W21">
         <v>41</v>
       </c>
       <c r="X21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z21">
         <v>0</v>
@@ -7652,16 +7652,16 @@
         <v>0</v>
       </c>
       <c r="BG21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK21">
         <v>22.08831486438843</v>
@@ -7676,10 +7676,10 @@
         <v>1.923868164652258</v>
       </c>
       <c r="BO21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ21">
         <v>1557.824413712093</v>
@@ -7759,16 +7759,16 @@
         <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22">
         <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F22">
         <v>15.406517900000001</v>
@@ -7804,10 +7804,10 @@
         <v>1.1637410400565691</v>
       </c>
       <c r="Q22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S22">
         <v>29</v>
@@ -7819,16 +7819,16 @@
         <v>100</v>
       </c>
       <c r="V22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W22">
         <v>34</v>
       </c>
       <c r="X22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z22">
         <v>0</v>
@@ -7930,16 +7930,16 @@
         <v>0</v>
       </c>
       <c r="BG22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK22">
         <v>23.800752898685118</v>
@@ -7954,10 +7954,10 @@
         <v>4.0833897722724384</v>
       </c>
       <c r="BO22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ22">
         <v>1304.034503704846</v>
@@ -8037,16 +8037,16 @@
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23">
         <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F23">
         <v>12.1942202</v>
@@ -8082,10 +8082,10 @@
         <v>1.5007581698119841</v>
       </c>
       <c r="Q23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S23">
         <v>31</v>
@@ -8097,16 +8097,16 @@
         <v>115</v>
       </c>
       <c r="V23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W23">
         <v>36</v>
       </c>
       <c r="X23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -8208,16 +8208,16 @@
         <v>0</v>
       </c>
       <c r="BG23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK23">
         <v>26.748680842065731</v>
@@ -8232,10 +8232,10 @@
         <v>2.5488088941415392</v>
       </c>
       <c r="BO23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ23">
         <v>1181.070752910847</v>
@@ -8315,16 +8315,16 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24">
         <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24">
         <v>14.1795966</v>
@@ -8360,10 +8360,10 @@
         <v>1.358783050394148</v>
       </c>
       <c r="Q24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S24">
         <v>32</v>
@@ -8375,16 +8375,16 @@
         <v>82</v>
       </c>
       <c r="V24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W24">
         <v>92</v>
       </c>
       <c r="X24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -8486,16 +8486,16 @@
         <v>0</v>
       </c>
       <c r="BG24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK24">
         <v>25.44395150418471</v>
@@ -8510,10 +8510,10 @@
         <v>3.7495788922281181</v>
       </c>
       <c r="BO24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ24">
         <v>1226.9980910723609</v>
@@ -8593,16 +8593,16 @@
         <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25">
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25">
         <v>4.06568533</v>
@@ -8638,10 +8638,10 @@
         <v>7.9651390121844301E-2</v>
       </c>
       <c r="Q25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S25">
         <v>13</v>
@@ -8653,16 +8653,16 @@
         <v>80</v>
       </c>
       <c r="V25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W25">
         <v>21</v>
       </c>
       <c r="X25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z25">
         <v>0</v>
@@ -8764,16 +8764,16 @@
         <v>0</v>
       </c>
       <c r="BG25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK25">
         <v>34.394535304590804</v>
@@ -8788,10 +8788,10 @@
         <v>23.550772197829598</v>
       </c>
       <c r="BO25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ25">
         <v>423.71127906536941</v>
@@ -8871,16 +8871,16 @@
         <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26">
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F26">
         <v>5.6505331500000002</v>
@@ -8916,10 +8916,10 @@
         <v>0.46658625178529428</v>
       </c>
       <c r="Q26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S26">
         <v>14</v>
@@ -8931,16 +8931,16 @@
         <v>72</v>
       </c>
       <c r="V26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W26">
         <v>14</v>
       </c>
       <c r="X26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z26">
         <v>0</v>
@@ -9042,16 +9042,16 @@
         <v>0</v>
       </c>
       <c r="BG26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK26">
         <v>32.89352154942658</v>
@@ -9066,10 +9066,10 @@
         <v>26.238610223104491</v>
       </c>
       <c r="BO26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ26">
         <v>463.14718254331439</v>
@@ -9149,16 +9149,16 @@
         <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27">
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F27">
         <v>4.0769583999999996</v>
@@ -9194,10 +9194,10 @@
         <v>0.25328761838530939</v>
       </c>
       <c r="Q27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S27">
         <v>15</v>
@@ -9209,16 +9209,16 @@
         <v>91</v>
       </c>
       <c r="V27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W27">
         <v>19</v>
       </c>
       <c r="X27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z27">
         <v>0</v>
@@ -9320,16 +9320,16 @@
         <v>0</v>
       </c>
       <c r="BG27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK27">
         <v>33.145466552929832</v>
@@ -9344,10 +9344,10 @@
         <v>23.28157426555974</v>
       </c>
       <c r="BO27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ27">
         <v>463.73686714236823</v>
@@ -9427,16 +9427,16 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28">
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F28">
         <v>12.405131600000001</v>
@@ -9472,10 +9472,10 @@
         <v>0.50146091540439564</v>
       </c>
       <c r="Q28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S28">
         <v>10</v>
@@ -9487,16 +9487,16 @@
         <v>83</v>
       </c>
       <c r="V28" t="s">
+        <v>132</v>
+      </c>
+      <c r="W28" t="s">
         <v>133</v>
       </c>
-      <c r="W28" t="s">
-        <v>134</v>
-      </c>
       <c r="X28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -9598,16 +9598,16 @@
         <v>0</v>
       </c>
       <c r="BG28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK28">
         <v>29.2243314984342</v>
@@ -9622,10 +9622,10 @@
         <v>25.908070790714991</v>
       </c>
       <c r="BO28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ28">
         <v>462.65948262028593</v>
@@ -9705,16 +9705,16 @@
         <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29">
         <v>7.8279325999999996</v>
@@ -9750,10 +9750,10 @@
         <v>0.8888695976695038</v>
       </c>
       <c r="Q29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S29">
         <v>2</v>
@@ -9765,16 +9765,16 @@
         <v>70</v>
       </c>
       <c r="V29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W29">
         <v>17</v>
       </c>
       <c r="X29" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y29" t="s">
         <v>132</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>133</v>
       </c>
       <c r="Z29">
         <v>0</v>
@@ -9876,16 +9876,16 @@
         <v>0</v>
       </c>
       <c r="BG29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK29">
         <v>36.513290823266409</v>
@@ -9900,10 +9900,10 @@
         <v>28.39665687393131</v>
       </c>
       <c r="BO29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ29">
         <v>383.34741258102628</v>
@@ -9983,16 +9983,16 @@
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F30">
         <v>5.6857524899999996</v>
@@ -10028,10 +10028,10 @@
         <v>1.0885361358368051</v>
       </c>
       <c r="Q30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S30">
         <v>6</v>
@@ -10043,16 +10043,16 @@
         <v>62</v>
       </c>
       <c r="V30" t="s">
+        <v>132</v>
+      </c>
+      <c r="W30" t="s">
         <v>133</v>
       </c>
-      <c r="W30" t="s">
-        <v>134</v>
-      </c>
       <c r="X30" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y30" t="s">
         <v>132</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>133</v>
       </c>
       <c r="Z30">
         <v>0</v>
@@ -10154,16 +10154,16 @@
         <v>0</v>
       </c>
       <c r="BG30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK30">
         <v>28.82697466537077</v>
@@ -10178,10 +10178,10 @@
         <v>30.480722401134958</v>
       </c>
       <c r="BO30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ30">
         <v>591.87278128818491</v>
@@ -10261,16 +10261,16 @@
         <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F31">
         <v>6.7176184299999999</v>
@@ -10306,10 +10306,10 @@
         <v>0.53763383277676446</v>
       </c>
       <c r="Q31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S31">
         <v>7</v>
@@ -10321,16 +10321,16 @@
         <v>61</v>
       </c>
       <c r="V31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W31">
         <v>70</v>
       </c>
       <c r="X31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z31">
         <v>0</v>
@@ -10432,16 +10432,16 @@
         <v>0</v>
       </c>
       <c r="BG31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BI31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BJ31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BK31">
         <v>35.366251150992071</v>
@@ -10456,10 +10456,10 @@
         <v>31.679159587710888</v>
       </c>
       <c r="BO31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BP31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BQ31">
         <v>573.23578017619377</v>

</xml_diff>

<commit_message>
Added doc strings for first 4 .py files
</commit_message>
<xml_diff>
--- a/docs/Examples/S6St_Testing/Muth_data_Merged.xlsx
+++ b/docs/Examples/S6St_Testing/Muth_data_Merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\docs\Examples\S6St_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0E506B-ADD0-4627-99D2-6D4E3324173E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFFABD7-BB42-4E5D-92A7-7B1F833BE83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,12 +55,6 @@
     <t>Centroid s.e.</t>
   </si>
   <si>
-    <t>Fe3+/∑ Fe</t>
-  </si>
-  <si>
-    <t>Fe3+/∑ Fe s.e.</t>
-  </si>
-  <si>
     <t>log (fO2)</t>
   </si>
   <si>
@@ -178,9 +172,6 @@
     <t>Unnamed: 37</t>
   </si>
   <si>
-    <t>1s.d.</t>
-  </si>
-  <si>
     <t>Unnamed: 40</t>
   </si>
   <si>
@@ -428,6 +419,15 @@
   </si>
   <si>
     <t>H2O_Liq</t>
+  </si>
+  <si>
+    <t>H2O_Liq_Err</t>
+  </si>
+  <si>
+    <t>Fe3Fet_Liq_Err</t>
+  </si>
+  <si>
+    <t>Fe3Fet_Liq</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CN31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1957,244 +1957,244 @@
         <v>10</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BD1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="CL1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CM1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="CN1" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:92" x14ac:dyDescent="0.35">
@@ -2202,16 +2202,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D2">
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F2">
         <v>27.025532599999998</v>
@@ -2247,10 +2247,10 @@
         <v>6.2229817769040352E-2</v>
       </c>
       <c r="Q2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S2">
         <v>32</v>
@@ -2262,16 +2262,16 @@
         <v>68</v>
       </c>
       <c r="V2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="W2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -2373,16 +2373,16 @@
         <v>0</v>
       </c>
       <c r="BG2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK2">
         <v>38.169542381598838</v>
@@ -2397,10 +2397,10 @@
         <v>3.7176611932427899</v>
       </c>
       <c r="BO2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ2">
         <v>329.01313474908687</v>
@@ -2480,16 +2480,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F3">
         <v>9.36523051</v>
@@ -2525,10 +2525,10 @@
         <v>0.91496216383051898</v>
       </c>
       <c r="Q3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S3">
         <v>33</v>
@@ -2540,16 +2540,16 @@
         <v>73</v>
       </c>
       <c r="V3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W3">
         <v>15</v>
       </c>
       <c r="X3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z3">
         <v>0</v>
@@ -2651,16 +2651,16 @@
         <v>0</v>
       </c>
       <c r="BG3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK3">
         <v>39.744192732047487</v>
@@ -2675,10 +2675,10 @@
         <v>4.5407213903284758</v>
       </c>
       <c r="BO3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ3">
         <v>344.95847330190611</v>
@@ -2758,16 +2758,16 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D4">
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F4">
         <v>14.9879231</v>
@@ -2803,10 +2803,10 @@
         <v>0.39548083233799319</v>
       </c>
       <c r="Q4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S4">
         <v>34</v>
@@ -2818,16 +2818,16 @@
         <v>70</v>
       </c>
       <c r="V4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -2929,106 +2929,106 @@
         <v>0</v>
       </c>
       <c r="BG4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BL4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BM4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BN4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BO4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BR4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BS4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BT4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BU4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BV4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BW4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BX4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BY4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BZ4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CA4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CB4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CC4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CD4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CE4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CF4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CG4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CH4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CI4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CJ4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CK4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CL4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CM4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="CN4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:92" x14ac:dyDescent="0.35">
@@ -3036,16 +3036,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5">
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <v>2.4291936299999999</v>
@@ -3081,10 +3081,10 @@
         <v>0.39169981916101371</v>
       </c>
       <c r="Q5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S5">
         <v>43</v>
@@ -3096,16 +3096,16 @@
         <v>99</v>
       </c>
       <c r="V5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="W5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z5">
         <v>0</v>
@@ -3207,16 +3207,16 @@
         <v>0</v>
       </c>
       <c r="BG5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK5">
         <v>38.023974689346772</v>
@@ -3231,10 +3231,10 @@
         <v>2.1747551134072109</v>
       </c>
       <c r="BO5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ5">
         <v>342.09419632057768</v>
@@ -3314,16 +3314,16 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D6">
         <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F6">
         <v>4.2422355100000004</v>
@@ -3359,10 +3359,10 @@
         <v>-0.1530333134115871</v>
       </c>
       <c r="Q6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S6">
         <v>44</v>
@@ -3374,16 +3374,16 @@
         <v>50</v>
       </c>
       <c r="V6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="W6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -3485,16 +3485,16 @@
         <v>0</v>
       </c>
       <c r="BG6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK6">
         <v>31.367362881690489</v>
@@ -3509,10 +3509,10 @@
         <v>3.7238699086723068</v>
       </c>
       <c r="BO6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ6">
         <v>267.48228796501462</v>
@@ -3592,16 +3592,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D7">
         <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F7">
         <v>3.46811231</v>
@@ -3637,10 +3637,10 @@
         <v>0.1873119834353574</v>
       </c>
       <c r="Q7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S7">
         <v>46</v>
@@ -3652,16 +3652,16 @@
         <v>68</v>
       </c>
       <c r="V7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W7">
         <v>17</v>
       </c>
       <c r="X7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -3763,16 +3763,16 @@
         <v>0</v>
       </c>
       <c r="BG7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK7">
         <v>37.000914935558988</v>
@@ -3787,10 +3787,10 @@
         <v>6.2567243500493666</v>
       </c>
       <c r="BO7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ7">
         <v>352.83423278792878</v>
@@ -3870,16 +3870,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D8">
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F8">
         <v>4.25856265</v>
@@ -3915,10 +3915,10 @@
         <v>0.13082012947838351</v>
       </c>
       <c r="Q8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S8">
         <v>47</v>
@@ -3930,16 +3930,16 @@
         <v>199</v>
       </c>
       <c r="V8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W8">
         <v>30</v>
       </c>
       <c r="X8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -4041,16 +4041,16 @@
         <v>0</v>
       </c>
       <c r="BG8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK8">
         <v>35.989276603544077</v>
@@ -4065,10 +4065,10 @@
         <v>2.638480034537606</v>
       </c>
       <c r="BO8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ8">
         <v>262.58828781622577</v>
@@ -4148,16 +4148,16 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9">
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F9">
         <v>3.0031961900000002</v>
@@ -4193,10 +4193,10 @@
         <v>0.72240736150953921</v>
       </c>
       <c r="Q9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S9">
         <v>49</v>
@@ -4208,16 +4208,16 @@
         <v>124</v>
       </c>
       <c r="V9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W9">
         <v>23</v>
       </c>
       <c r="X9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z9">
         <v>0</v>
@@ -4319,16 +4319,16 @@
         <v>0</v>
       </c>
       <c r="BG9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK9">
         <v>35.521029871422598</v>
@@ -4343,10 +4343,10 @@
         <v>3.890594072974686</v>
       </c>
       <c r="BO9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ9">
         <v>416.17366923363198</v>
@@ -4426,16 +4426,16 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10">
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F10">
         <v>10.5209841</v>
@@ -4471,10 +4471,10 @@
         <v>1.687700667581425</v>
       </c>
       <c r="Q10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S10">
         <v>31</v>
@@ -4486,16 +4486,16 @@
         <v>142</v>
       </c>
       <c r="V10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -4597,16 +4597,16 @@
         <v>0</v>
       </c>
       <c r="BG10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK10">
         <v>29.21396749938555</v>
@@ -4621,10 +4621,10 @@
         <v>3.609883869529853</v>
       </c>
       <c r="BO10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ10">
         <v>547.31158362190047</v>
@@ -4704,16 +4704,16 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D11">
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F11">
         <v>12.515108100000001</v>
@@ -4749,10 +4749,10 @@
         <v>0.59070339497109092</v>
       </c>
       <c r="Q11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S11">
         <v>35</v>
@@ -4764,16 +4764,16 @@
         <v>105</v>
       </c>
       <c r="V11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W11">
         <v>30</v>
       </c>
       <c r="X11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z11">
         <v>0</v>
@@ -4860,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="BC11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BD11">
         <v>0</v>
@@ -4872,16 +4872,16 @@
         <v>0</v>
       </c>
       <c r="BG11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK11">
         <v>28.20679628271272</v>
@@ -4896,10 +4896,10 @@
         <v>22.59307037763795</v>
       </c>
       <c r="BO11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ11">
         <v>611.21828981207409</v>
@@ -4979,16 +4979,16 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F12">
         <v>14.1435382</v>
@@ -5024,10 +5024,10 @@
         <v>1.181562344963744</v>
       </c>
       <c r="Q12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S12">
         <v>37</v>
@@ -5039,16 +5039,16 @@
         <v>175</v>
       </c>
       <c r="V12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W12">
         <v>43</v>
       </c>
       <c r="X12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z12">
         <v>0</v>
@@ -5150,16 +5150,16 @@
         <v>0</v>
       </c>
       <c r="BG12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK12">
         <v>26.63579698290221</v>
@@ -5174,10 +5174,10 @@
         <v>22.44700736875712</v>
       </c>
       <c r="BO12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ12">
         <v>598.20829930660295</v>
@@ -5257,16 +5257,16 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D13">
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F13">
         <v>15.5100181</v>
@@ -5302,10 +5302,10 @@
         <v>0.93441137034893718</v>
       </c>
       <c r="Q13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S13">
         <v>40</v>
@@ -5317,16 +5317,16 @@
         <v>106</v>
       </c>
       <c r="V13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W13">
         <v>12</v>
       </c>
       <c r="X13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -5428,16 +5428,16 @@
         <v>0</v>
       </c>
       <c r="BG13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK13">
         <v>29.645304229912</v>
@@ -5452,10 +5452,10 @@
         <v>2.7735406262329252</v>
       </c>
       <c r="BO13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ13">
         <v>502.62986375819838</v>
@@ -5535,16 +5535,16 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D14">
         <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F14">
         <v>10.2321428</v>
@@ -5580,10 +5580,10 @@
         <v>0.45103082329631938</v>
       </c>
       <c r="Q14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S14">
         <v>42</v>
@@ -5595,16 +5595,16 @@
         <v>157</v>
       </c>
       <c r="V14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W14">
         <v>33</v>
       </c>
       <c r="X14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z14">
         <v>0</v>
@@ -5706,16 +5706,16 @@
         <v>0</v>
       </c>
       <c r="BG14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK14">
         <v>29.850978444450451</v>
@@ -5730,10 +5730,10 @@
         <v>2.52588408913565</v>
       </c>
       <c r="BO14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ14">
         <v>509.02639760211707</v>
@@ -5813,16 +5813,16 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D15">
         <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F15">
         <v>24.687177399999999</v>
@@ -5858,10 +5858,10 @@
         <v>0.84496962264111541</v>
       </c>
       <c r="Q15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S15">
         <v>43</v>
@@ -5873,16 +5873,16 @@
         <v>182</v>
       </c>
       <c r="V15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W15">
         <v>36</v>
       </c>
       <c r="X15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z15">
         <v>0</v>
@@ -5984,16 +5984,16 @@
         <v>0</v>
       </c>
       <c r="BG15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK15">
         <v>26.47064138546795</v>
@@ -6008,10 +6008,10 @@
         <v>1.9088966431122181</v>
       </c>
       <c r="BO15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ15">
         <v>547.75275620552577</v>
@@ -6091,16 +6091,16 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D16">
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F16">
         <v>19.833613400000001</v>
@@ -6136,10 +6136,10 @@
         <v>1.0178894787784061</v>
       </c>
       <c r="Q16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S16">
         <v>44</v>
@@ -6151,16 +6151,16 @@
         <v>124</v>
       </c>
       <c r="V16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W16">
         <v>37</v>
       </c>
       <c r="X16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z16">
         <v>0</v>
@@ -6262,16 +6262,16 @@
         <v>0</v>
       </c>
       <c r="BG16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK16">
         <v>32.1982185018257</v>
@@ -6286,10 +6286,10 @@
         <v>3.5169220839420241</v>
       </c>
       <c r="BO16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ16">
         <v>594.33645723496352</v>
@@ -6369,16 +6369,16 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D17">
         <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F17">
         <v>15.7119658</v>
@@ -6414,10 +6414,10 @@
         <v>1.201499415607985</v>
       </c>
       <c r="Q17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S17">
         <v>45</v>
@@ -6429,16 +6429,16 @@
         <v>103</v>
       </c>
       <c r="V17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W17">
         <v>26</v>
       </c>
       <c r="X17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -6540,16 +6540,16 @@
         <v>0</v>
       </c>
       <c r="BG17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK17">
         <v>27.957828990121499</v>
@@ -6564,10 +6564,10 @@
         <v>2.4854242886727569</v>
       </c>
       <c r="BO17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ17">
         <v>504.38328682330058</v>
@@ -6647,16 +6647,16 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18">
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F18">
         <v>28.259062700000001</v>
@@ -6692,10 +6692,10 @@
         <v>1.981462480172594</v>
       </c>
       <c r="Q18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="S18">
         <v>34</v>
@@ -6707,16 +6707,16 @@
         <v>83</v>
       </c>
       <c r="V18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W18">
         <v>25</v>
       </c>
       <c r="X18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z18">
         <v>0</v>
@@ -6818,16 +6818,16 @@
         <v>0</v>
       </c>
       <c r="BG18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK18">
         <v>24.944217453532001</v>
@@ -6842,10 +6842,10 @@
         <v>5.1132634054668129</v>
       </c>
       <c r="BO18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ18">
         <v>1364.1140703829931</v>
@@ -6925,16 +6925,16 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D19">
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F19">
         <v>17.500456499999999</v>
@@ -6970,10 +6970,10 @@
         <v>1.513325575930268</v>
       </c>
       <c r="Q19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S19">
         <v>24</v>
@@ -6985,16 +6985,16 @@
         <v>133</v>
       </c>
       <c r="V19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W19">
         <v>41</v>
       </c>
       <c r="X19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -7096,16 +7096,16 @@
         <v>0</v>
       </c>
       <c r="BG19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK19">
         <v>26.880975495325028</v>
@@ -7120,10 +7120,10 @@
         <v>2.0821057028422851</v>
       </c>
       <c r="BO19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ19">
         <v>1158.8975882102111</v>
@@ -7203,16 +7203,16 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D20">
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F20">
         <v>16.568765800000001</v>
@@ -7248,10 +7248,10 @@
         <v>1.5280233808882939</v>
       </c>
       <c r="Q20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S20">
         <v>25</v>
@@ -7263,16 +7263,16 @@
         <v>144</v>
       </c>
       <c r="V20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W20">
         <v>38</v>
       </c>
       <c r="X20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z20">
         <v>0</v>
@@ -7374,16 +7374,16 @@
         <v>0</v>
       </c>
       <c r="BG20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK20">
         <v>22.87165538428523</v>
@@ -7398,10 +7398,10 @@
         <v>2.3652605950055769</v>
       </c>
       <c r="BO20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ20">
         <v>1431.3457870844061</v>
@@ -7481,16 +7481,16 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D21">
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F21">
         <v>13.236040900000001</v>
@@ -7526,10 +7526,10 @@
         <v>1.315035136481066</v>
       </c>
       <c r="Q21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S21">
         <v>26</v>
@@ -7541,16 +7541,16 @@
         <v>109</v>
       </c>
       <c r="V21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W21">
         <v>41</v>
       </c>
       <c r="X21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z21">
         <v>0</v>
@@ -7652,16 +7652,16 @@
         <v>0</v>
       </c>
       <c r="BG21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK21">
         <v>22.08831486438843</v>
@@ -7676,10 +7676,10 @@
         <v>1.923868164652258</v>
       </c>
       <c r="BO21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ21">
         <v>1557.824413712093</v>
@@ -7759,16 +7759,16 @@
         <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D22">
         <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F22">
         <v>15.406517900000001</v>
@@ -7804,10 +7804,10 @@
         <v>1.1637410400565691</v>
       </c>
       <c r="Q22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S22">
         <v>29</v>
@@ -7819,16 +7819,16 @@
         <v>100</v>
       </c>
       <c r="V22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W22">
         <v>34</v>
       </c>
       <c r="X22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z22">
         <v>0</v>
@@ -7930,16 +7930,16 @@
         <v>0</v>
       </c>
       <c r="BG22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK22">
         <v>23.800752898685118</v>
@@ -7954,10 +7954,10 @@
         <v>4.0833897722724384</v>
       </c>
       <c r="BO22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ22">
         <v>1304.034503704846</v>
@@ -8037,16 +8037,16 @@
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D23">
         <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F23">
         <v>12.1942202</v>
@@ -8082,10 +8082,10 @@
         <v>1.5007581698119841</v>
       </c>
       <c r="Q23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S23">
         <v>31</v>
@@ -8097,16 +8097,16 @@
         <v>115</v>
       </c>
       <c r="V23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W23">
         <v>36</v>
       </c>
       <c r="X23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -8208,16 +8208,16 @@
         <v>0</v>
       </c>
       <c r="BG23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK23">
         <v>26.748680842065731</v>
@@ -8232,10 +8232,10 @@
         <v>2.5488088941415392</v>
       </c>
       <c r="BO23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ23">
         <v>1181.070752910847</v>
@@ -8315,16 +8315,16 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D24">
         <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F24">
         <v>14.1795966</v>
@@ -8360,10 +8360,10 @@
         <v>1.358783050394148</v>
       </c>
       <c r="Q24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S24">
         <v>32</v>
@@ -8375,16 +8375,16 @@
         <v>82</v>
       </c>
       <c r="V24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W24">
         <v>92</v>
       </c>
       <c r="X24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -8486,16 +8486,16 @@
         <v>0</v>
       </c>
       <c r="BG24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK24">
         <v>25.44395150418471</v>
@@ -8510,10 +8510,10 @@
         <v>3.7495788922281181</v>
       </c>
       <c r="BO24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ24">
         <v>1226.9980910723609</v>
@@ -8593,16 +8593,16 @@
         <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D25">
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F25">
         <v>4.06568533</v>
@@ -8638,10 +8638,10 @@
         <v>7.9651390121844301E-2</v>
       </c>
       <c r="Q25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S25">
         <v>13</v>
@@ -8653,16 +8653,16 @@
         <v>80</v>
       </c>
       <c r="V25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W25">
         <v>21</v>
       </c>
       <c r="X25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z25">
         <v>0</v>
@@ -8764,16 +8764,16 @@
         <v>0</v>
       </c>
       <c r="BG25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK25">
         <v>34.394535304590804</v>
@@ -8788,10 +8788,10 @@
         <v>23.550772197829598</v>
       </c>
       <c r="BO25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ25">
         <v>423.71127906536941</v>
@@ -8871,16 +8871,16 @@
         <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D26">
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F26">
         <v>5.6505331500000002</v>
@@ -8916,10 +8916,10 @@
         <v>0.46658625178529428</v>
       </c>
       <c r="Q26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S26">
         <v>14</v>
@@ -8931,16 +8931,16 @@
         <v>72</v>
       </c>
       <c r="V26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W26">
         <v>14</v>
       </c>
       <c r="X26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z26">
         <v>0</v>
@@ -9042,16 +9042,16 @@
         <v>0</v>
       </c>
       <c r="BG26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK26">
         <v>32.89352154942658</v>
@@ -9066,10 +9066,10 @@
         <v>26.238610223104491</v>
       </c>
       <c r="BO26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ26">
         <v>463.14718254331439</v>
@@ -9149,16 +9149,16 @@
         <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D27">
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F27">
         <v>4.0769583999999996</v>
@@ -9194,10 +9194,10 @@
         <v>0.25328761838530939</v>
       </c>
       <c r="Q27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S27">
         <v>15</v>
@@ -9209,16 +9209,16 @@
         <v>91</v>
       </c>
       <c r="V27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W27">
         <v>19</v>
       </c>
       <c r="X27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z27">
         <v>0</v>
@@ -9320,16 +9320,16 @@
         <v>0</v>
       </c>
       <c r="BG27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK27">
         <v>33.145466552929832</v>
@@ -9344,10 +9344,10 @@
         <v>23.28157426555974</v>
       </c>
       <c r="BO27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ27">
         <v>463.73686714236823</v>
@@ -9427,16 +9427,16 @@
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D28">
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F28">
         <v>12.405131600000001</v>
@@ -9472,10 +9472,10 @@
         <v>0.50146091540439564</v>
       </c>
       <c r="Q28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S28">
         <v>10</v>
@@ -9487,16 +9487,16 @@
         <v>83</v>
       </c>
       <c r="V28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -9598,16 +9598,16 @@
         <v>0</v>
       </c>
       <c r="BG28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK28">
         <v>29.2243314984342</v>
@@ -9622,10 +9622,10 @@
         <v>25.908070790714991</v>
       </c>
       <c r="BO28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ28">
         <v>462.65948262028593</v>
@@ -9705,16 +9705,16 @@
         <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F29">
         <v>7.8279325999999996</v>
@@ -9750,10 +9750,10 @@
         <v>0.8888695976695038</v>
       </c>
       <c r="Q29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S29">
         <v>2</v>
@@ -9765,16 +9765,16 @@
         <v>70</v>
       </c>
       <c r="V29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W29">
         <v>17</v>
       </c>
       <c r="X29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z29">
         <v>0</v>
@@ -9876,16 +9876,16 @@
         <v>0</v>
       </c>
       <c r="BG29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK29">
         <v>36.513290823266409</v>
@@ -9900,10 +9900,10 @@
         <v>28.39665687393131</v>
       </c>
       <c r="BO29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ29">
         <v>383.34741258102628</v>
@@ -9983,16 +9983,16 @@
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D30">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F30">
         <v>5.6857524899999996</v>
@@ -10028,10 +10028,10 @@
         <v>1.0885361358368051</v>
       </c>
       <c r="Q30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S30">
         <v>6</v>
@@ -10043,16 +10043,16 @@
         <v>62</v>
       </c>
       <c r="V30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z30">
         <v>0</v>
@@ -10154,16 +10154,16 @@
         <v>0</v>
       </c>
       <c r="BG30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK30">
         <v>28.82697466537077</v>
@@ -10178,10 +10178,10 @@
         <v>30.480722401134958</v>
       </c>
       <c r="BO30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ30">
         <v>591.87278128818491</v>
@@ -10261,16 +10261,16 @@
         <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D31">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F31">
         <v>6.7176184299999999</v>
@@ -10306,10 +10306,10 @@
         <v>0.53763383277676446</v>
       </c>
       <c r="Q31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S31">
         <v>7</v>
@@ -10321,16 +10321,16 @@
         <v>61</v>
       </c>
       <c r="V31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W31">
         <v>70</v>
       </c>
       <c r="X31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z31">
         <v>0</v>
@@ -10432,16 +10432,16 @@
         <v>0</v>
       </c>
       <c r="BG31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BH31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BI31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BJ31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BK31">
         <v>35.366251150992071</v>
@@ -10456,10 +10456,10 @@
         <v>31.679159587710888</v>
       </c>
       <c r="BO31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BP31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BQ31">
         <v>573.23578017619377</v>

</xml_diff>